<commit_message>
Terminar Parser de Dataset Excel -> JSON. Para futura lectura y compartir con otros equipos.
</commit_message>
<xml_diff>
--- a/dataset/Clustered.xlsx
+++ b/dataset/Clustered.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MultipleLayerPerceptron\dataset\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -60,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,20 +491,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -508,6 +504,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,12 +525,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -567,7 +575,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,9 +608,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,6 +660,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -810,19 +852,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="BD57" sqref="BD57:BF68"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.5546875" style="7"/>
+    <col min="1" max="16384" width="11.5703125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>-1</v>
       </c>
@@ -1013,7 +1055,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>-1</v>
       </c>
@@ -1204,7 +1246,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>-1</v>
       </c>
@@ -1395,7 +1437,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>-1</v>
       </c>
@@ -1586,7 +1628,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>-1</v>
       </c>
@@ -1777,7 +1819,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>-1</v>
       </c>
@@ -1968,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>-1</v>
       </c>
@@ -2159,7 +2201,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>-1</v>
       </c>
@@ -2350,7 +2392,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:63" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>1</v>
       </c>
@@ -2541,7 +2583,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>-1</v>
       </c>
@@ -2732,7 +2774,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>-1</v>
       </c>
@@ -2923,7 +2965,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>-1</v>
       </c>
@@ -3114,7 +3156,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>-1</v>
       </c>
@@ -3305,7 +3347,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>-1</v>
       </c>
@@ -3496,7 +3538,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>-1</v>
       </c>
@@ -3687,7 +3729,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>-1</v>
       </c>
@@ -3878,7 +3920,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>-1</v>
       </c>
@@ -4069,7 +4111,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:63" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="24">
         <v>-1</v>
       </c>
@@ -4260,7 +4302,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="28">
         <v>-1</v>
       </c>
@@ -4451,7 +4493,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="32">
         <v>-1</v>
       </c>
@@ -4512,7 +4554,9 @@
       <c r="T20" s="56">
         <v>-1</v>
       </c>
-      <c r="U20" s="56"/>
+      <c r="U20" s="56">
+        <v>-1</v>
+      </c>
       <c r="V20" s="56">
         <v>1</v>
       </c>
@@ -4640,7 +4684,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="32">
         <v>-1</v>
       </c>
@@ -4740,7 +4784,9 @@
       <c r="AG21" s="164">
         <v>1</v>
       </c>
-      <c r="AH21" s="164"/>
+      <c r="AH21" s="195">
+        <v>-1</v>
+      </c>
       <c r="AI21" s="164">
         <v>-1</v>
       </c>
@@ -4829,7 +4875,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="32">
         <v>-1</v>
       </c>
@@ -5020,7 +5066,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="32">
         <v>-1</v>
       </c>
@@ -5211,7 +5257,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="32">
         <v>-1</v>
       </c>
@@ -5402,7 +5448,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="32">
         <v>-1</v>
       </c>
@@ -5593,7 +5639,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="32">
         <v>-1</v>
       </c>
@@ -5690,7 +5736,9 @@
       <c r="AF26" s="164">
         <v>1</v>
       </c>
-      <c r="AG26" s="164"/>
+      <c r="AG26" s="195">
+        <v>1</v>
+      </c>
       <c r="AH26" s="164">
         <v>-1</v>
       </c>
@@ -5782,7 +5830,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:63" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="34">
         <v>-1</v>
       </c>
@@ -5973,7 +6021,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="166">
         <v>-1</v>
       </c>
@@ -6164,7 +6212,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="169">
         <v>-1</v>
       </c>
@@ -6355,7 +6403,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="169">
         <v>-1</v>
       </c>
@@ -6546,7 +6594,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="169">
         <v>-1</v>
       </c>
@@ -6737,7 +6785,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="169">
         <v>-1</v>
       </c>
@@ -6928,7 +6976,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="169">
         <v>-1</v>
       </c>
@@ -7119,7 +7167,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="169">
         <v>-1</v>
       </c>
@@ -7310,7 +7358,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="169">
         <v>1</v>
       </c>
@@ -7356,7 +7404,9 @@
       <c r="O35" s="178">
         <v>1</v>
       </c>
-      <c r="P35" s="178"/>
+      <c r="P35" s="195">
+        <v>-1</v>
+      </c>
       <c r="Q35" s="178">
         <v>-1</v>
       </c>
@@ -7499,7 +7549,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:63" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="172">
         <v>-1</v>
       </c>
@@ -7690,7 +7740,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="166">
         <v>-1</v>
       </c>
@@ -7881,7 +7931,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="169">
         <v>-1</v>
       </c>
@@ -7942,7 +7992,9 @@
       <c r="T38" s="185">
         <v>-1</v>
       </c>
-      <c r="U38" s="185"/>
+      <c r="U38" s="195">
+        <v>-1</v>
+      </c>
       <c r="V38" s="185">
         <v>1</v>
       </c>
@@ -8070,7 +8122,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="169">
         <v>-1</v>
       </c>
@@ -8261,7 +8313,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="169">
         <v>-1</v>
       </c>
@@ -8452,7 +8504,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="169">
         <v>-1</v>
       </c>
@@ -8643,7 +8695,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="169">
         <v>1</v>
       </c>
@@ -8834,7 +8886,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="169">
         <v>-1</v>
       </c>
@@ -9025,7 +9077,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:63" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="169">
         <v>-1</v>
       </c>
@@ -9216,7 +9268,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:63" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:63" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="172">
         <v>1</v>
       </c>
@@ -9407,7 +9459,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:63" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="166">
         <v>-1</v>
       </c>
@@ -9445,7 +9497,7 @@
         <v>1</v>
       </c>
       <c r="M46" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N46" s="167">
         <v>1</v>
@@ -9469,10 +9521,10 @@
         <v>-1</v>
       </c>
       <c r="U46" s="167">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V46" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="W46" s="167">
         <v>-1</v>
@@ -9502,7 +9554,7 @@
         <v>1</v>
       </c>
       <c r="AF46" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AG46" s="167">
         <v>1</v>
@@ -9520,7 +9572,7 @@
         <v>-1</v>
       </c>
       <c r="AL46" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AM46" s="167">
         <v>1</v>
@@ -9532,10 +9584,10 @@
         <v>1</v>
       </c>
       <c r="AP46" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AQ46" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR46" s="167">
         <v>-1</v>
@@ -9550,16 +9602,16 @@
         <v>1</v>
       </c>
       <c r="AV46" s="167">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW46" s="167">
         <v>1</v>
       </c>
       <c r="AX46" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AY46" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AZ46" s="167">
         <v>1</v>
@@ -9583,7 +9635,7 @@
         <v>1</v>
       </c>
       <c r="BG46" s="167">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BH46" s="167">
         <v>1</v>
@@ -9598,29 +9650,29 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:63" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="169">
         <v>-1</v>
       </c>
       <c r="B47" s="177">
         <v>-1</v>
       </c>
-      <c r="C47" s="177">
-        <v>-1</v>
-      </c>
-      <c r="D47" s="177">
-        <v>1</v>
-      </c>
-      <c r="E47" s="177">
-        <v>1</v>
-      </c>
-      <c r="F47" s="177">
-        <v>1</v>
-      </c>
-      <c r="G47" s="177">
-        <v>-1</v>
-      </c>
-      <c r="H47" s="177">
+      <c r="C47" s="194">
+        <v>-1</v>
+      </c>
+      <c r="D47" s="194">
+        <v>1</v>
+      </c>
+      <c r="E47" s="194">
+        <v>1</v>
+      </c>
+      <c r="F47" s="194">
+        <v>1</v>
+      </c>
+      <c r="G47" s="194">
+        <v>-1</v>
+      </c>
+      <c r="H47" s="194">
         <v>-1</v>
       </c>
       <c r="I47" s="171">
@@ -9629,7 +9681,7 @@
       <c r="J47" s="169">
         <v>-1</v>
       </c>
-      <c r="K47" s="189">
+      <c r="K47" s="194">
         <v>1</v>
       </c>
       <c r="L47" s="189">
@@ -9789,29 +9841,29 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:63" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="169">
         <v>-1</v>
       </c>
       <c r="B48" s="177">
         <v>-1</v>
       </c>
-      <c r="C48" s="177">
-        <v>-1</v>
-      </c>
-      <c r="D48" s="177">
-        <v>1</v>
-      </c>
-      <c r="E48" s="177">
-        <v>-1</v>
-      </c>
-      <c r="F48" s="177">
-        <v>1</v>
-      </c>
-      <c r="G48" s="177">
-        <v>-1</v>
-      </c>
-      <c r="H48" s="177">
+      <c r="C48" s="194">
+        <v>-1</v>
+      </c>
+      <c r="D48" s="194">
+        <v>1</v>
+      </c>
+      <c r="E48" s="194">
+        <v>-1</v>
+      </c>
+      <c r="F48" s="194">
+        <v>1</v>
+      </c>
+      <c r="G48" s="194">
+        <v>-1</v>
+      </c>
+      <c r="H48" s="194">
         <v>-1</v>
       </c>
       <c r="I48" s="171">
@@ -9820,7 +9872,7 @@
       <c r="J48" s="169">
         <v>-1</v>
       </c>
-      <c r="K48" s="189">
+      <c r="K48" s="194">
         <v>1</v>
       </c>
       <c r="L48" s="189">
@@ -9929,7 +9981,7 @@
         <v>-1</v>
       </c>
       <c r="AU48" s="192">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AV48" s="192">
         <v>-1</v>
@@ -9980,29 +10032,29 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:63" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="169">
         <v>-1</v>
       </c>
       <c r="B49" s="177">
         <v>-1</v>
       </c>
-      <c r="C49" s="177">
-        <v>1</v>
-      </c>
-      <c r="D49" s="177">
-        <v>1</v>
-      </c>
-      <c r="E49" s="177">
-        <v>-1</v>
-      </c>
-      <c r="F49" s="177">
-        <v>1</v>
-      </c>
-      <c r="G49" s="177">
-        <v>1</v>
-      </c>
-      <c r="H49" s="177">
+      <c r="C49" s="194">
+        <v>1</v>
+      </c>
+      <c r="D49" s="194">
+        <v>1</v>
+      </c>
+      <c r="E49" s="194">
+        <v>-1</v>
+      </c>
+      <c r="F49" s="194">
+        <v>1</v>
+      </c>
+      <c r="G49" s="194">
+        <v>0</v>
+      </c>
+      <c r="H49" s="194">
         <v>-1</v>
       </c>
       <c r="I49" s="171">
@@ -10011,7 +10063,7 @@
       <c r="J49" s="169">
         <v>-1</v>
       </c>
-      <c r="K49" s="189">
+      <c r="K49" s="194">
         <v>1</v>
       </c>
       <c r="L49" s="189">
@@ -10039,7 +10091,7 @@
         <v>-1</v>
       </c>
       <c r="T49" s="189">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="U49" s="189">
         <v>-1</v>
@@ -10066,7 +10118,7 @@
         <v>-1</v>
       </c>
       <c r="AC49" s="190">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD49" s="190">
         <v>-1</v>
@@ -10084,7 +10136,7 @@
         <v>-1</v>
       </c>
       <c r="AI49" s="190">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ49" s="171">
         <v>-1</v>
@@ -10171,29 +10223,29 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:63" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="169">
         <v>-1</v>
       </c>
       <c r="B50" s="177">
         <v>-1</v>
       </c>
-      <c r="C50" s="177">
-        <v>1</v>
-      </c>
-      <c r="D50" s="177">
-        <v>-1</v>
-      </c>
-      <c r="E50" s="177">
-        <v>-1</v>
-      </c>
-      <c r="F50" s="177">
-        <v>-1</v>
-      </c>
-      <c r="G50" s="177">
-        <v>-1</v>
-      </c>
-      <c r="H50" s="177">
+      <c r="C50" s="194">
+        <v>1</v>
+      </c>
+      <c r="D50" s="194">
+        <v>-1</v>
+      </c>
+      <c r="E50" s="194">
+        <v>-1</v>
+      </c>
+      <c r="F50" s="194">
+        <v>-1</v>
+      </c>
+      <c r="G50" s="194">
+        <v>-1</v>
+      </c>
+      <c r="H50" s="194">
         <v>-1</v>
       </c>
       <c r="I50" s="171">
@@ -10202,17 +10254,17 @@
       <c r="J50" s="169">
         <v>-1</v>
       </c>
-      <c r="K50" s="189">
+      <c r="K50" s="194">
         <v>1</v>
       </c>
       <c r="L50" s="189">
         <v>1</v>
       </c>
       <c r="M50" s="189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N50" s="189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O50" s="189">
         <v>1</v>
@@ -10221,7 +10273,7 @@
         <v>1</v>
       </c>
       <c r="Q50" s="189">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R50" s="171">
         <v>-1</v>
@@ -10275,7 +10327,7 @@
         <v>-1</v>
       </c>
       <c r="AI50" s="190">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AJ50" s="171">
         <v>-1</v>
@@ -10290,7 +10342,7 @@
         <v>1</v>
       </c>
       <c r="AN50" s="191">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AO50" s="191">
         <v>1</v>
@@ -10362,29 +10414,29 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:63" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="169">
         <v>-1</v>
       </c>
       <c r="B51" s="177">
         <v>-1</v>
       </c>
-      <c r="C51" s="177">
-        <v>1</v>
-      </c>
-      <c r="D51" s="177">
-        <v>-1</v>
-      </c>
-      <c r="E51" s="177">
-        <v>-1</v>
-      </c>
-      <c r="F51" s="177">
-        <v>-1</v>
-      </c>
-      <c r="G51" s="177">
-        <v>1</v>
-      </c>
-      <c r="H51" s="177">
+      <c r="C51" s="194">
+        <v>1</v>
+      </c>
+      <c r="D51" s="194">
+        <v>-1</v>
+      </c>
+      <c r="E51" s="194">
+        <v>-1</v>
+      </c>
+      <c r="F51" s="194">
+        <v>-1</v>
+      </c>
+      <c r="G51" s="194">
+        <v>0</v>
+      </c>
+      <c r="H51" s="194">
         <v>-1</v>
       </c>
       <c r="I51" s="171">
@@ -10393,7 +10445,7 @@
       <c r="J51" s="169">
         <v>-1</v>
       </c>
-      <c r="K51" s="189">
+      <c r="K51" s="194">
         <v>1</v>
       </c>
       <c r="L51" s="189">
@@ -10529,7 +10581,7 @@
         <v>-1</v>
       </c>
       <c r="BD51" s="193">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BE51" s="193">
         <v>-1</v>
@@ -10547,35 +10599,35 @@
         <v>-1</v>
       </c>
       <c r="BJ51" s="193">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BK51" s="171">
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:63" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="169">
         <v>-1</v>
       </c>
       <c r="B52" s="177">
         <v>1</v>
       </c>
-      <c r="C52" s="177">
-        <v>1</v>
-      </c>
-      <c r="D52" s="177">
-        <v>1</v>
-      </c>
-      <c r="E52" s="177">
-        <v>1</v>
-      </c>
-      <c r="F52" s="177">
-        <v>1</v>
-      </c>
-      <c r="G52" s="177">
-        <v>-1</v>
-      </c>
-      <c r="H52" s="177">
+      <c r="C52" s="194">
+        <v>1</v>
+      </c>
+      <c r="D52" s="194">
+        <v>1</v>
+      </c>
+      <c r="E52" s="194">
+        <v>0</v>
+      </c>
+      <c r="F52" s="194">
+        <v>1</v>
+      </c>
+      <c r="G52" s="194">
+        <v>-1</v>
+      </c>
+      <c r="H52" s="194">
         <v>1</v>
       </c>
       <c r="I52" s="171">
@@ -10584,8 +10636,8 @@
       <c r="J52" s="169">
         <v>-1</v>
       </c>
-      <c r="K52" s="189">
-        <v>-1</v>
+      <c r="K52" s="194">
+        <v>0</v>
       </c>
       <c r="L52" s="189">
         <v>-1</v>
@@ -10603,7 +10655,7 @@
         <v>-1</v>
       </c>
       <c r="Q52" s="189">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="R52" s="171">
         <v>-1</v>
@@ -10612,7 +10664,7 @@
         <v>-1</v>
       </c>
       <c r="T52" s="189">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="U52" s="189">
         <v>-1</v>
@@ -10639,7 +10691,7 @@
         <v>-1</v>
       </c>
       <c r="AC52" s="190">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD52" s="190">
         <v>-1</v>
@@ -10738,35 +10790,35 @@
         <v>-1</v>
       </c>
       <c r="BJ52" s="193">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="BK52" s="171">
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:63" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:63" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="169">
         <v>-1</v>
       </c>
       <c r="B53" s="177">
         <v>1</v>
       </c>
-      <c r="C53" s="177">
-        <v>-1</v>
-      </c>
-      <c r="D53" s="177">
-        <v>-1</v>
-      </c>
-      <c r="E53" s="177">
-        <v>-1</v>
-      </c>
-      <c r="F53" s="177">
-        <v>-1</v>
-      </c>
-      <c r="G53" s="177">
-        <v>-1</v>
-      </c>
-      <c r="H53" s="177">
+      <c r="C53" s="194">
+        <v>-1</v>
+      </c>
+      <c r="D53" s="194">
+        <v>-1</v>
+      </c>
+      <c r="E53" s="194">
+        <v>-1</v>
+      </c>
+      <c r="F53" s="194">
+        <v>-1</v>
+      </c>
+      <c r="G53" s="194">
+        <v>-1</v>
+      </c>
+      <c r="H53" s="194">
         <v>1</v>
       </c>
       <c r="I53" s="171">
@@ -10775,7 +10827,7 @@
       <c r="J53" s="169">
         <v>-1</v>
       </c>
-      <c r="K53" s="189">
+      <c r="K53" s="194">
         <v>1</v>
       </c>
       <c r="L53" s="189">
@@ -10803,7 +10855,7 @@
         <v>-1</v>
       </c>
       <c r="T53" s="189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U53" s="189">
         <v>-1</v>
@@ -10884,7 +10936,7 @@
         <v>-1</v>
       </c>
       <c r="AU53" s="192">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AV53" s="192">
         <v>-1</v>
@@ -10935,7 +10987,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:63" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:63" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="172">
         <v>-1</v>
       </c>
@@ -10973,7 +11025,7 @@
         <v>1</v>
       </c>
       <c r="M54" s="173">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N54" s="173">
         <v>1</v>
@@ -11003,7 +11055,7 @@
         <v>1</v>
       </c>
       <c r="W54" s="173">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="X54" s="173">
         <v>1</v>
@@ -11027,7 +11079,7 @@
         <v>1</v>
       </c>
       <c r="AE54" s="173">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AF54" s="173">
         <v>1</v>
@@ -11048,7 +11100,7 @@
         <v>-1</v>
       </c>
       <c r="AL54" s="173">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AM54" s="173">
         <v>1</v>
@@ -11060,10 +11112,10 @@
         <v>1</v>
       </c>
       <c r="AP54" s="173">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AQ54" s="173">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AR54" s="173">
         <v>-1</v>
@@ -11126,547 +11178,547 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B57" s="197" t="s">
+    <row r="57" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B57" s="202" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="197"/>
-      <c r="D57" s="197"/>
-      <c r="E57" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="F57" s="196"/>
-      <c r="K57" s="198" t="s">
+      <c r="C57" s="202"/>
+      <c r="D57" s="202"/>
+      <c r="E57" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="197"/>
+      <c r="K57" s="203" t="s">
         <v>7</v>
       </c>
-      <c r="L57" s="198"/>
-      <c r="M57" s="198"/>
-      <c r="N57" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="O57" s="196"/>
-      <c r="U57" s="199" t="s">
+      <c r="L57" s="203"/>
+      <c r="M57" s="203"/>
+      <c r="N57" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="O57" s="197"/>
+      <c r="U57" s="196" t="s">
         <v>8</v>
       </c>
-      <c r="V57" s="199"/>
-      <c r="W57" s="199"/>
-      <c r="X57" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y57" s="196"/>
-      <c r="AC57" s="201" t="s">
+      <c r="V57" s="196"/>
+      <c r="W57" s="196"/>
+      <c r="X57" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y57" s="197"/>
+      <c r="AC57" s="198" t="s">
         <v>9</v>
       </c>
-      <c r="AD57" s="201"/>
-      <c r="AE57" s="201"/>
-      <c r="AF57" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG57" s="196"/>
-      <c r="AL57" s="202" t="s">
+      <c r="AD57" s="198"/>
+      <c r="AE57" s="198"/>
+      <c r="AF57" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG57" s="197"/>
+      <c r="AL57" s="199" t="s">
         <v>10</v>
       </c>
-      <c r="AM57" s="202"/>
-      <c r="AN57" s="202"/>
-      <c r="AO57" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP57" s="196"/>
-      <c r="AU57" s="203" t="s">
+      <c r="AM57" s="199"/>
+      <c r="AN57" s="199"/>
+      <c r="AO57" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP57" s="197"/>
+      <c r="AU57" s="200" t="s">
         <v>11</v>
       </c>
-      <c r="AV57" s="203"/>
-      <c r="AW57" s="203"/>
-      <c r="AX57" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="AY57" s="196"/>
-      <c r="BD57" s="200" t="s">
+      <c r="AV57" s="200"/>
+      <c r="AW57" s="200"/>
+      <c r="AX57" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY57" s="197"/>
+      <c r="BD57" s="201" t="s">
         <v>12</v>
       </c>
-      <c r="BE57" s="200"/>
-      <c r="BF57" s="200"/>
-      <c r="BG57" s="196" t="s">
-        <v>1</v>
-      </c>
-      <c r="BH57" s="196"/>
+      <c r="BE57" s="201"/>
+      <c r="BF57" s="201"/>
+      <c r="BG57" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="BH57" s="197"/>
     </row>
-    <row r="58" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B58" s="197"/>
-      <c r="C58" s="197"/>
-      <c r="D58" s="197"/>
-      <c r="E58" s="196"/>
-      <c r="F58" s="196"/>
-      <c r="K58" s="198"/>
-      <c r="L58" s="198"/>
-      <c r="M58" s="198"/>
-      <c r="N58" s="196"/>
-      <c r="O58" s="196"/>
-      <c r="U58" s="199"/>
-      <c r="V58" s="199"/>
-      <c r="W58" s="199"/>
-      <c r="X58" s="196"/>
-      <c r="Y58" s="196"/>
-      <c r="AC58" s="201"/>
-      <c r="AD58" s="201"/>
-      <c r="AE58" s="201"/>
-      <c r="AF58" s="196"/>
-      <c r="AG58" s="196"/>
-      <c r="AL58" s="202"/>
-      <c r="AM58" s="202"/>
-      <c r="AN58" s="202"/>
-      <c r="AO58" s="196"/>
-      <c r="AP58" s="196"/>
-      <c r="AU58" s="203"/>
-      <c r="AV58" s="203"/>
-      <c r="AW58" s="203"/>
-      <c r="AX58" s="196"/>
-      <c r="AY58" s="196"/>
-      <c r="BD58" s="200"/>
-      <c r="BE58" s="200"/>
-      <c r="BF58" s="200"/>
-      <c r="BG58" s="196"/>
-      <c r="BH58" s="196"/>
+    <row r="58" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B58" s="202"/>
+      <c r="C58" s="202"/>
+      <c r="D58" s="202"/>
+      <c r="E58" s="197"/>
+      <c r="F58" s="197"/>
+      <c r="K58" s="203"/>
+      <c r="L58" s="203"/>
+      <c r="M58" s="203"/>
+      <c r="N58" s="197"/>
+      <c r="O58" s="197"/>
+      <c r="U58" s="196"/>
+      <c r="V58" s="196"/>
+      <c r="W58" s="196"/>
+      <c r="X58" s="197"/>
+      <c r="Y58" s="197"/>
+      <c r="AC58" s="198"/>
+      <c r="AD58" s="198"/>
+      <c r="AE58" s="198"/>
+      <c r="AF58" s="197"/>
+      <c r="AG58" s="197"/>
+      <c r="AL58" s="199"/>
+      <c r="AM58" s="199"/>
+      <c r="AN58" s="199"/>
+      <c r="AO58" s="197"/>
+      <c r="AP58" s="197"/>
+      <c r="AU58" s="200"/>
+      <c r="AV58" s="200"/>
+      <c r="AW58" s="200"/>
+      <c r="AX58" s="197"/>
+      <c r="AY58" s="197"/>
+      <c r="BD58" s="201"/>
+      <c r="BE58" s="201"/>
+      <c r="BF58" s="201"/>
+      <c r="BG58" s="197"/>
+      <c r="BH58" s="197"/>
     </row>
-    <row r="59" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B59" s="197"/>
-      <c r="C59" s="197"/>
-      <c r="D59" s="197"/>
-      <c r="E59" s="196" t="s">
+    <row r="59" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B59" s="202"/>
+      <c r="C59" s="202"/>
+      <c r="D59" s="202"/>
+      <c r="E59" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="F59" s="196"/>
-      <c r="K59" s="198"/>
-      <c r="L59" s="198"/>
-      <c r="M59" s="198"/>
-      <c r="N59" s="196" t="s">
+      <c r="F59" s="197"/>
+      <c r="K59" s="203"/>
+      <c r="L59" s="203"/>
+      <c r="M59" s="203"/>
+      <c r="N59" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="O59" s="196"/>
-      <c r="U59" s="199"/>
-      <c r="V59" s="199"/>
-      <c r="W59" s="199"/>
-      <c r="X59" s="196" t="s">
+      <c r="O59" s="197"/>
+      <c r="U59" s="196"/>
+      <c r="V59" s="196"/>
+      <c r="W59" s="196"/>
+      <c r="X59" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="Y59" s="196"/>
-      <c r="AC59" s="201"/>
-      <c r="AD59" s="201"/>
-      <c r="AE59" s="201"/>
-      <c r="AF59" s="196" t="s">
+      <c r="Y59" s="197"/>
+      <c r="AC59" s="198"/>
+      <c r="AD59" s="198"/>
+      <c r="AE59" s="198"/>
+      <c r="AF59" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="AG59" s="196"/>
-      <c r="AL59" s="202"/>
-      <c r="AM59" s="202"/>
-      <c r="AN59" s="202"/>
-      <c r="AO59" s="196" t="s">
+      <c r="AG59" s="197"/>
+      <c r="AL59" s="199"/>
+      <c r="AM59" s="199"/>
+      <c r="AN59" s="199"/>
+      <c r="AO59" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="AP59" s="196"/>
-      <c r="AU59" s="203"/>
-      <c r="AV59" s="203"/>
-      <c r="AW59" s="203"/>
-      <c r="AX59" s="196" t="s">
+      <c r="AP59" s="197"/>
+      <c r="AU59" s="200"/>
+      <c r="AV59" s="200"/>
+      <c r="AW59" s="200"/>
+      <c r="AX59" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="AY59" s="196"/>
-      <c r="BD59" s="200"/>
-      <c r="BE59" s="200"/>
-      <c r="BF59" s="200"/>
-      <c r="BG59" s="196" t="s">
+      <c r="AY59" s="197"/>
+      <c r="BD59" s="201"/>
+      <c r="BE59" s="201"/>
+      <c r="BF59" s="201"/>
+      <c r="BG59" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="BH59" s="196"/>
+      <c r="BH59" s="197"/>
     </row>
-    <row r="60" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B60" s="197"/>
-      <c r="C60" s="197"/>
-      <c r="D60" s="197"/>
-      <c r="E60" s="196"/>
-      <c r="F60" s="196"/>
-      <c r="K60" s="198"/>
-      <c r="L60" s="198"/>
-      <c r="M60" s="198"/>
-      <c r="N60" s="196"/>
-      <c r="O60" s="196"/>
-      <c r="U60" s="199"/>
-      <c r="V60" s="199"/>
-      <c r="W60" s="199"/>
-      <c r="X60" s="196"/>
-      <c r="Y60" s="196"/>
-      <c r="AC60" s="201"/>
-      <c r="AD60" s="201"/>
-      <c r="AE60" s="201"/>
-      <c r="AF60" s="196"/>
-      <c r="AG60" s="196"/>
-      <c r="AL60" s="202"/>
-      <c r="AM60" s="202"/>
-      <c r="AN60" s="202"/>
-      <c r="AO60" s="196"/>
-      <c r="AP60" s="196"/>
-      <c r="AU60" s="203"/>
-      <c r="AV60" s="203"/>
-      <c r="AW60" s="203"/>
-      <c r="AX60" s="196"/>
-      <c r="AY60" s="196"/>
-      <c r="BD60" s="200"/>
-      <c r="BE60" s="200"/>
-      <c r="BF60" s="200"/>
-      <c r="BG60" s="196"/>
-      <c r="BH60" s="196"/>
+    <row r="60" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B60" s="202"/>
+      <c r="C60" s="202"/>
+      <c r="D60" s="202"/>
+      <c r="E60" s="197"/>
+      <c r="F60" s="197"/>
+      <c r="K60" s="203"/>
+      <c r="L60" s="203"/>
+      <c r="M60" s="203"/>
+      <c r="N60" s="197"/>
+      <c r="O60" s="197"/>
+      <c r="U60" s="196"/>
+      <c r="V60" s="196"/>
+      <c r="W60" s="196"/>
+      <c r="X60" s="197"/>
+      <c r="Y60" s="197"/>
+      <c r="AC60" s="198"/>
+      <c r="AD60" s="198"/>
+      <c r="AE60" s="198"/>
+      <c r="AF60" s="197"/>
+      <c r="AG60" s="197"/>
+      <c r="AL60" s="199"/>
+      <c r="AM60" s="199"/>
+      <c r="AN60" s="199"/>
+      <c r="AO60" s="197"/>
+      <c r="AP60" s="197"/>
+      <c r="AU60" s="200"/>
+      <c r="AV60" s="200"/>
+      <c r="AW60" s="200"/>
+      <c r="AX60" s="197"/>
+      <c r="AY60" s="197"/>
+      <c r="BD60" s="201"/>
+      <c r="BE60" s="201"/>
+      <c r="BF60" s="201"/>
+      <c r="BG60" s="197"/>
+      <c r="BH60" s="197"/>
     </row>
-    <row r="61" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B61" s="197"/>
-      <c r="C61" s="197"/>
-      <c r="D61" s="197"/>
-      <c r="E61" s="196" t="s">
+    <row r="61" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B61" s="202"/>
+      <c r="C61" s="202"/>
+      <c r="D61" s="202"/>
+      <c r="E61" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="F61" s="196"/>
-      <c r="K61" s="198"/>
-      <c r="L61" s="198"/>
-      <c r="M61" s="198"/>
-      <c r="N61" s="196" t="s">
+      <c r="F61" s="197"/>
+      <c r="K61" s="203"/>
+      <c r="L61" s="203"/>
+      <c r="M61" s="203"/>
+      <c r="N61" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="O61" s="196"/>
-      <c r="U61" s="199"/>
-      <c r="V61" s="199"/>
-      <c r="W61" s="199"/>
-      <c r="X61" s="196" t="s">
+      <c r="O61" s="197"/>
+      <c r="U61" s="196"/>
+      <c r="V61" s="196"/>
+      <c r="W61" s="196"/>
+      <c r="X61" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="Y61" s="196"/>
-      <c r="AC61" s="201"/>
-      <c r="AD61" s="201"/>
-      <c r="AE61" s="201"/>
-      <c r="AF61" s="196" t="s">
+      <c r="Y61" s="197"/>
+      <c r="AC61" s="198"/>
+      <c r="AD61" s="198"/>
+      <c r="AE61" s="198"/>
+      <c r="AF61" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="AG61" s="196"/>
-      <c r="AL61" s="202"/>
-      <c r="AM61" s="202"/>
-      <c r="AN61" s="202"/>
-      <c r="AO61" s="196" t="s">
+      <c r="AG61" s="197"/>
+      <c r="AL61" s="199"/>
+      <c r="AM61" s="199"/>
+      <c r="AN61" s="199"/>
+      <c r="AO61" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="AP61" s="196"/>
-      <c r="AU61" s="203"/>
-      <c r="AV61" s="203"/>
-      <c r="AW61" s="203"/>
-      <c r="AX61" s="196" t="s">
+      <c r="AP61" s="197"/>
+      <c r="AU61" s="200"/>
+      <c r="AV61" s="200"/>
+      <c r="AW61" s="200"/>
+      <c r="AX61" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="AY61" s="196"/>
-      <c r="BD61" s="200"/>
-      <c r="BE61" s="200"/>
-      <c r="BF61" s="200"/>
-      <c r="BG61" s="196" t="s">
+      <c r="AY61" s="197"/>
+      <c r="BD61" s="201"/>
+      <c r="BE61" s="201"/>
+      <c r="BF61" s="201"/>
+      <c r="BG61" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="BH61" s="196"/>
+      <c r="BH61" s="197"/>
     </row>
-    <row r="62" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B62" s="197"/>
-      <c r="C62" s="197"/>
-      <c r="D62" s="197"/>
-      <c r="E62" s="196"/>
-      <c r="F62" s="196"/>
-      <c r="K62" s="198"/>
-      <c r="L62" s="198"/>
-      <c r="M62" s="198"/>
-      <c r="N62" s="196"/>
-      <c r="O62" s="196"/>
-      <c r="U62" s="199"/>
-      <c r="V62" s="199"/>
-      <c r="W62" s="199"/>
-      <c r="X62" s="196"/>
-      <c r="Y62" s="196"/>
-      <c r="AC62" s="201"/>
-      <c r="AD62" s="201"/>
-      <c r="AE62" s="201"/>
-      <c r="AF62" s="196"/>
-      <c r="AG62" s="196"/>
-      <c r="AL62" s="202"/>
-      <c r="AM62" s="202"/>
-      <c r="AN62" s="202"/>
-      <c r="AO62" s="196"/>
-      <c r="AP62" s="196"/>
-      <c r="AU62" s="203"/>
-      <c r="AV62" s="203"/>
-      <c r="AW62" s="203"/>
-      <c r="AX62" s="196"/>
-      <c r="AY62" s="196"/>
-      <c r="BD62" s="200"/>
-      <c r="BE62" s="200"/>
-      <c r="BF62" s="200"/>
-      <c r="BG62" s="196"/>
-      <c r="BH62" s="196"/>
+    <row r="62" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B62" s="202"/>
+      <c r="C62" s="202"/>
+      <c r="D62" s="202"/>
+      <c r="E62" s="197"/>
+      <c r="F62" s="197"/>
+      <c r="K62" s="203"/>
+      <c r="L62" s="203"/>
+      <c r="M62" s="203"/>
+      <c r="N62" s="197"/>
+      <c r="O62" s="197"/>
+      <c r="U62" s="196"/>
+      <c r="V62" s="196"/>
+      <c r="W62" s="196"/>
+      <c r="X62" s="197"/>
+      <c r="Y62" s="197"/>
+      <c r="AC62" s="198"/>
+      <c r="AD62" s="198"/>
+      <c r="AE62" s="198"/>
+      <c r="AF62" s="197"/>
+      <c r="AG62" s="197"/>
+      <c r="AL62" s="199"/>
+      <c r="AM62" s="199"/>
+      <c r="AN62" s="199"/>
+      <c r="AO62" s="197"/>
+      <c r="AP62" s="197"/>
+      <c r="AU62" s="200"/>
+      <c r="AV62" s="200"/>
+      <c r="AW62" s="200"/>
+      <c r="AX62" s="197"/>
+      <c r="AY62" s="197"/>
+      <c r="BD62" s="201"/>
+      <c r="BE62" s="201"/>
+      <c r="BF62" s="201"/>
+      <c r="BG62" s="197"/>
+      <c r="BH62" s="197"/>
     </row>
-    <row r="63" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B63" s="197"/>
-      <c r="C63" s="197"/>
-      <c r="D63" s="197"/>
-      <c r="E63" s="196" t="s">
+    <row r="63" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B63" s="202"/>
+      <c r="C63" s="202"/>
+      <c r="D63" s="202"/>
+      <c r="E63" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="196"/>
-      <c r="K63" s="198"/>
-      <c r="L63" s="198"/>
-      <c r="M63" s="198"/>
-      <c r="N63" s="196" t="s">
+      <c r="F63" s="197"/>
+      <c r="K63" s="203"/>
+      <c r="L63" s="203"/>
+      <c r="M63" s="203"/>
+      <c r="N63" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="O63" s="196"/>
-      <c r="U63" s="199"/>
-      <c r="V63" s="199"/>
-      <c r="W63" s="199"/>
-      <c r="X63" s="196" t="s">
+      <c r="O63" s="197"/>
+      <c r="U63" s="196"/>
+      <c r="V63" s="196"/>
+      <c r="W63" s="196"/>
+      <c r="X63" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="Y63" s="196"/>
-      <c r="AC63" s="201"/>
-      <c r="AD63" s="201"/>
-      <c r="AE63" s="201"/>
-      <c r="AF63" s="196" t="s">
+      <c r="Y63" s="197"/>
+      <c r="AC63" s="198"/>
+      <c r="AD63" s="198"/>
+      <c r="AE63" s="198"/>
+      <c r="AF63" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="AG63" s="196"/>
-      <c r="AL63" s="202"/>
-      <c r="AM63" s="202"/>
-      <c r="AN63" s="202"/>
-      <c r="AO63" s="196" t="s">
+      <c r="AG63" s="197"/>
+      <c r="AL63" s="199"/>
+      <c r="AM63" s="199"/>
+      <c r="AN63" s="199"/>
+      <c r="AO63" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="AP63" s="196"/>
-      <c r="AU63" s="203"/>
-      <c r="AV63" s="203"/>
-      <c r="AW63" s="203"/>
-      <c r="AX63" s="196" t="s">
+      <c r="AP63" s="197"/>
+      <c r="AU63" s="200"/>
+      <c r="AV63" s="200"/>
+      <c r="AW63" s="200"/>
+      <c r="AX63" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="AY63" s="196"/>
-      <c r="BD63" s="200"/>
-      <c r="BE63" s="200"/>
-      <c r="BF63" s="200"/>
-      <c r="BG63" s="196" t="s">
+      <c r="AY63" s="197"/>
+      <c r="BD63" s="201"/>
+      <c r="BE63" s="201"/>
+      <c r="BF63" s="201"/>
+      <c r="BG63" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="BH63" s="196"/>
+      <c r="BH63" s="197"/>
     </row>
-    <row r="64" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="B64" s="197"/>
-      <c r="C64" s="197"/>
-      <c r="D64" s="197"/>
-      <c r="E64" s="196"/>
-      <c r="F64" s="196"/>
-      <c r="K64" s="198"/>
-      <c r="L64" s="198"/>
-      <c r="M64" s="198"/>
-      <c r="N64" s="196"/>
-      <c r="O64" s="196"/>
-      <c r="U64" s="199"/>
-      <c r="V64" s="199"/>
-      <c r="W64" s="199"/>
-      <c r="X64" s="196"/>
-      <c r="Y64" s="196"/>
-      <c r="AC64" s="201"/>
-      <c r="AD64" s="201"/>
-      <c r="AE64" s="201"/>
-      <c r="AF64" s="196"/>
-      <c r="AG64" s="196"/>
-      <c r="AL64" s="202"/>
-      <c r="AM64" s="202"/>
-      <c r="AN64" s="202"/>
-      <c r="AO64" s="196"/>
-      <c r="AP64" s="196"/>
-      <c r="AU64" s="203"/>
-      <c r="AV64" s="203"/>
-      <c r="AW64" s="203"/>
-      <c r="AX64" s="196"/>
-      <c r="AY64" s="196"/>
-      <c r="BD64" s="200"/>
-      <c r="BE64" s="200"/>
-      <c r="BF64" s="200"/>
-      <c r="BG64" s="196"/>
-      <c r="BH64" s="196"/>
+    <row r="64" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B64" s="202"/>
+      <c r="C64" s="202"/>
+      <c r="D64" s="202"/>
+      <c r="E64" s="197"/>
+      <c r="F64" s="197"/>
+      <c r="K64" s="203"/>
+      <c r="L64" s="203"/>
+      <c r="M64" s="203"/>
+      <c r="N64" s="197"/>
+      <c r="O64" s="197"/>
+      <c r="U64" s="196"/>
+      <c r="V64" s="196"/>
+      <c r="W64" s="196"/>
+      <c r="X64" s="197"/>
+      <c r="Y64" s="197"/>
+      <c r="AC64" s="198"/>
+      <c r="AD64" s="198"/>
+      <c r="AE64" s="198"/>
+      <c r="AF64" s="197"/>
+      <c r="AG64" s="197"/>
+      <c r="AL64" s="199"/>
+      <c r="AM64" s="199"/>
+      <c r="AN64" s="199"/>
+      <c r="AO64" s="197"/>
+      <c r="AP64" s="197"/>
+      <c r="AU64" s="200"/>
+      <c r="AV64" s="200"/>
+      <c r="AW64" s="200"/>
+      <c r="AX64" s="197"/>
+      <c r="AY64" s="197"/>
+      <c r="BD64" s="201"/>
+      <c r="BE64" s="201"/>
+      <c r="BF64" s="201"/>
+      <c r="BG64" s="197"/>
+      <c r="BH64" s="197"/>
     </row>
-    <row r="65" spans="2:60" x14ac:dyDescent="0.3">
-      <c r="B65" s="197"/>
-      <c r="C65" s="197"/>
-      <c r="D65" s="197"/>
-      <c r="E65" s="196" t="s">
+    <row r="65" spans="2:60" x14ac:dyDescent="0.25">
+      <c r="B65" s="202"/>
+      <c r="C65" s="202"/>
+      <c r="D65" s="202"/>
+      <c r="E65" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="196"/>
-      <c r="K65" s="198"/>
-      <c r="L65" s="198"/>
-      <c r="M65" s="198"/>
-      <c r="N65" s="196" t="s">
+      <c r="F65" s="197"/>
+      <c r="K65" s="203"/>
+      <c r="L65" s="203"/>
+      <c r="M65" s="203"/>
+      <c r="N65" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="O65" s="196"/>
-      <c r="U65" s="199"/>
-      <c r="V65" s="199"/>
-      <c r="W65" s="199"/>
-      <c r="X65" s="196" t="s">
+      <c r="O65" s="197"/>
+      <c r="U65" s="196"/>
+      <c r="V65" s="196"/>
+      <c r="W65" s="196"/>
+      <c r="X65" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="Y65" s="196"/>
-      <c r="AC65" s="201"/>
-      <c r="AD65" s="201"/>
-      <c r="AE65" s="201"/>
-      <c r="AF65" s="196" t="s">
+      <c r="Y65" s="197"/>
+      <c r="AC65" s="198"/>
+      <c r="AD65" s="198"/>
+      <c r="AE65" s="198"/>
+      <c r="AF65" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="AG65" s="196"/>
-      <c r="AL65" s="202"/>
-      <c r="AM65" s="202"/>
-      <c r="AN65" s="202"/>
-      <c r="AO65" s="196" t="s">
+      <c r="AG65" s="197"/>
+      <c r="AL65" s="199"/>
+      <c r="AM65" s="199"/>
+      <c r="AN65" s="199"/>
+      <c r="AO65" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="AP65" s="196"/>
-      <c r="AU65" s="203"/>
-      <c r="AV65" s="203"/>
-      <c r="AW65" s="203"/>
-      <c r="AX65" s="196" t="s">
+      <c r="AP65" s="197"/>
+      <c r="AU65" s="200"/>
+      <c r="AV65" s="200"/>
+      <c r="AW65" s="200"/>
+      <c r="AX65" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="AY65" s="196"/>
-      <c r="BD65" s="200"/>
-      <c r="BE65" s="200"/>
-      <c r="BF65" s="200"/>
-      <c r="BG65" s="196" t="s">
+      <c r="AY65" s="197"/>
+      <c r="BD65" s="201"/>
+      <c r="BE65" s="201"/>
+      <c r="BF65" s="201"/>
+      <c r="BG65" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="BH65" s="196"/>
+      <c r="BH65" s="197"/>
     </row>
-    <row r="66" spans="2:60" x14ac:dyDescent="0.3">
-      <c r="B66" s="197"/>
-      <c r="C66" s="197"/>
-      <c r="D66" s="197"/>
-      <c r="E66" s="196"/>
-      <c r="F66" s="196"/>
-      <c r="K66" s="198"/>
-      <c r="L66" s="198"/>
-      <c r="M66" s="198"/>
-      <c r="N66" s="196"/>
-      <c r="O66" s="196"/>
-      <c r="U66" s="199"/>
-      <c r="V66" s="199"/>
-      <c r="W66" s="199"/>
-      <c r="X66" s="196"/>
-      <c r="Y66" s="196"/>
-      <c r="AC66" s="201"/>
-      <c r="AD66" s="201"/>
-      <c r="AE66" s="201"/>
-      <c r="AF66" s="196"/>
-      <c r="AG66" s="196"/>
-      <c r="AL66" s="202"/>
-      <c r="AM66" s="202"/>
-      <c r="AN66" s="202"/>
-      <c r="AO66" s="196"/>
-      <c r="AP66" s="196"/>
-      <c r="AU66" s="203"/>
-      <c r="AV66" s="203"/>
-      <c r="AW66" s="203"/>
-      <c r="AX66" s="196"/>
-      <c r="AY66" s="196"/>
-      <c r="BD66" s="200"/>
-      <c r="BE66" s="200"/>
-      <c r="BF66" s="200"/>
-      <c r="BG66" s="196"/>
-      <c r="BH66" s="196"/>
+    <row r="66" spans="2:60" x14ac:dyDescent="0.25">
+      <c r="B66" s="202"/>
+      <c r="C66" s="202"/>
+      <c r="D66" s="202"/>
+      <c r="E66" s="197"/>
+      <c r="F66" s="197"/>
+      <c r="K66" s="203"/>
+      <c r="L66" s="203"/>
+      <c r="M66" s="203"/>
+      <c r="N66" s="197"/>
+      <c r="O66" s="197"/>
+      <c r="U66" s="196"/>
+      <c r="V66" s="196"/>
+      <c r="W66" s="196"/>
+      <c r="X66" s="197"/>
+      <c r="Y66" s="197"/>
+      <c r="AC66" s="198"/>
+      <c r="AD66" s="198"/>
+      <c r="AE66" s="198"/>
+      <c r="AF66" s="197"/>
+      <c r="AG66" s="197"/>
+      <c r="AL66" s="199"/>
+      <c r="AM66" s="199"/>
+      <c r="AN66" s="199"/>
+      <c r="AO66" s="197"/>
+      <c r="AP66" s="197"/>
+      <c r="AU66" s="200"/>
+      <c r="AV66" s="200"/>
+      <c r="AW66" s="200"/>
+      <c r="AX66" s="197"/>
+      <c r="AY66" s="197"/>
+      <c r="BD66" s="201"/>
+      <c r="BE66" s="201"/>
+      <c r="BF66" s="201"/>
+      <c r="BG66" s="197"/>
+      <c r="BH66" s="197"/>
     </row>
-    <row r="67" spans="2:60" x14ac:dyDescent="0.3">
-      <c r="B67" s="197"/>
-      <c r="C67" s="197"/>
-      <c r="D67" s="197"/>
-      <c r="E67" s="196" t="s">
+    <row r="67" spans="2:60" x14ac:dyDescent="0.25">
+      <c r="B67" s="202"/>
+      <c r="C67" s="202"/>
+      <c r="D67" s="202"/>
+      <c r="E67" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="F67" s="196"/>
-      <c r="K67" s="198"/>
-      <c r="L67" s="198"/>
-      <c r="M67" s="198"/>
-      <c r="N67" s="196" t="s">
+      <c r="F67" s="197"/>
+      <c r="K67" s="203"/>
+      <c r="L67" s="203"/>
+      <c r="M67" s="203"/>
+      <c r="N67" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="O67" s="196"/>
-      <c r="U67" s="199"/>
-      <c r="V67" s="199"/>
-      <c r="W67" s="199"/>
-      <c r="X67" s="196" t="s">
+      <c r="O67" s="197"/>
+      <c r="U67" s="196"/>
+      <c r="V67" s="196"/>
+      <c r="W67" s="196"/>
+      <c r="X67" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="Y67" s="196"/>
-      <c r="AC67" s="201"/>
-      <c r="AD67" s="201"/>
-      <c r="AE67" s="201"/>
-      <c r="AF67" s="196" t="s">
+      <c r="Y67" s="197"/>
+      <c r="AC67" s="198"/>
+      <c r="AD67" s="198"/>
+      <c r="AE67" s="198"/>
+      <c r="AF67" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="AG67" s="196"/>
-      <c r="AL67" s="202"/>
-      <c r="AM67" s="202"/>
-      <c r="AN67" s="202"/>
-      <c r="AO67" s="196" t="s">
+      <c r="AG67" s="197"/>
+      <c r="AL67" s="199"/>
+      <c r="AM67" s="199"/>
+      <c r="AN67" s="199"/>
+      <c r="AO67" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="AP67" s="196"/>
-      <c r="AU67" s="203"/>
-      <c r="AV67" s="203"/>
-      <c r="AW67" s="203"/>
-      <c r="AX67" s="196" t="s">
+      <c r="AP67" s="197"/>
+      <c r="AU67" s="200"/>
+      <c r="AV67" s="200"/>
+      <c r="AW67" s="200"/>
+      <c r="AX67" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="AY67" s="196"/>
-      <c r="BD67" s="200"/>
-      <c r="BE67" s="200"/>
-      <c r="BF67" s="200"/>
-      <c r="BG67" s="196" t="s">
+      <c r="AY67" s="197"/>
+      <c r="BD67" s="201"/>
+      <c r="BE67" s="201"/>
+      <c r="BF67" s="201"/>
+      <c r="BG67" s="197" t="s">
         <v>6</v>
       </c>
-      <c r="BH67" s="196"/>
+      <c r="BH67" s="197"/>
     </row>
-    <row r="68" spans="2:60" x14ac:dyDescent="0.3">
-      <c r="B68" s="197"/>
-      <c r="C68" s="197"/>
-      <c r="D68" s="197"/>
-      <c r="E68" s="196"/>
-      <c r="F68" s="196"/>
-      <c r="K68" s="198"/>
-      <c r="L68" s="198"/>
-      <c r="M68" s="198"/>
-      <c r="N68" s="196"/>
-      <c r="O68" s="196"/>
-      <c r="U68" s="199"/>
-      <c r="V68" s="199"/>
-      <c r="W68" s="199"/>
-      <c r="X68" s="196"/>
-      <c r="Y68" s="196"/>
-      <c r="AC68" s="201"/>
-      <c r="AD68" s="201"/>
-      <c r="AE68" s="201"/>
-      <c r="AF68" s="196"/>
-      <c r="AG68" s="196"/>
-      <c r="AL68" s="202"/>
-      <c r="AM68" s="202"/>
-      <c r="AN68" s="202"/>
-      <c r="AO68" s="196"/>
-      <c r="AP68" s="196"/>
-      <c r="AU68" s="203"/>
-      <c r="AV68" s="203"/>
-      <c r="AW68" s="203"/>
-      <c r="AX68" s="196"/>
-      <c r="AY68" s="196"/>
-      <c r="BD68" s="200"/>
-      <c r="BE68" s="200"/>
-      <c r="BF68" s="200"/>
-      <c r="BG68" s="196"/>
-      <c r="BH68" s="196"/>
+    <row r="68" spans="2:60" x14ac:dyDescent="0.25">
+      <c r="B68" s="202"/>
+      <c r="C68" s="202"/>
+      <c r="D68" s="202"/>
+      <c r="E68" s="197"/>
+      <c r="F68" s="197"/>
+      <c r="K68" s="203"/>
+      <c r="L68" s="203"/>
+      <c r="M68" s="203"/>
+      <c r="N68" s="197"/>
+      <c r="O68" s="197"/>
+      <c r="U68" s="196"/>
+      <c r="V68" s="196"/>
+      <c r="W68" s="196"/>
+      <c r="X68" s="197"/>
+      <c r="Y68" s="197"/>
+      <c r="AC68" s="198"/>
+      <c r="AD68" s="198"/>
+      <c r="AE68" s="198"/>
+      <c r="AF68" s="197"/>
+      <c r="AG68" s="197"/>
+      <c r="AL68" s="199"/>
+      <c r="AM68" s="199"/>
+      <c r="AN68" s="199"/>
+      <c r="AO68" s="197"/>
+      <c r="AP68" s="197"/>
+      <c r="AU68" s="200"/>
+      <c r="AV68" s="200"/>
+      <c r="AW68" s="200"/>
+      <c r="AX68" s="197"/>
+      <c r="AY68" s="197"/>
+      <c r="BD68" s="201"/>
+      <c r="BE68" s="201"/>
+      <c r="BF68" s="201"/>
+      <c r="BG68" s="197"/>
+      <c r="BH68" s="197"/>
     </row>
   </sheetData>
   <mergeCells count="49">
@@ -11726,24 +11778,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>